<commit_message>
reorganize, re-run strategy results
</commit_message>
<xml_diff>
--- a/parameter_files/base/entity_list.xlsx
+++ b/parameter_files/base/entity_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="29" documentId="8_{9B5B270A-A4B1-448C-A90D-73D5A1A125A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{944BBDA8-09C4-4FE4-A66D-919188DD7692}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{48D6A96F-44BE-4B70-8FC3-216E0C53B229}"/>
+    <workbookView minimized="1" xWindow="2770" yWindow="1290" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{48D6A96F-44BE-4B70-8FC3-216E0C53B229}"/>
   </bookViews>
   <sheets>
     <sheet name="N" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>